<commit_message>
test both fixed waterlevel types
</commit_message>
<xml_diff>
--- a/test/data/full_test.xlsx
+++ b/test/data/full_test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dupuits\Documents\probabilistic_piping\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99F4C26-10B7-42CC-BC48-B096F38C7802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E6CA03-05C9-44C7-A6AC-A630402B03E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="1995" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{AE50B85C-D6AF-4F25-9D04-EA25405220D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AE50B85C-D6AF-4F25-9D04-EA25405220D2}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
-    <sheet name="output" sheetId="1" r:id="rId2"/>
+    <sheet name="output" sheetId="3" r:id="rId2"/>
+    <sheet name="output_simple" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="93">
   <si>
     <t>waterstand</t>
   </si>
@@ -897,7 +898,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,11 +1963,1646 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756F92DD-9D0B-402C-A237-40551468B067}">
+  <dimension ref="A1:B202"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25">
+        <v>1.955537683050252E-32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="25">
+        <v>1.020085182974381E-31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="B4" s="25">
+        <v>5.3517509293792589E-31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="B5" s="25">
+        <v>2.8204838175960761E-30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>1.4912633834011451E-29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="25">
+        <v>7.8986008680652674E-29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="B8" s="25">
+        <v>4.1839277191507523E-28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="B9" s="25">
+        <v>2.2122596799035069E-27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1.165193678904387E-26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="B11" s="25">
+        <v>6.0994215645407976E-26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>1</v>
+      </c>
+      <c r="B12" s="25">
+        <v>3.168289213741792E-25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B13" s="25">
+        <v>1.9184780879605411E-25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="B14" s="25">
+        <v>8.1645682560512982E-24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>1.3</v>
+      </c>
+      <c r="B15" s="25">
+        <v>4.0733632046727392E-23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>1.4</v>
+      </c>
+      <c r="B16" s="25">
+        <v>1.9953389729240051E-22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="B17" s="25">
+        <v>9.5751089244126588E-22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>1.6</v>
+      </c>
+      <c r="B18" s="25">
+        <v>4.4918200392331792E-21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>1.7</v>
+      </c>
+      <c r="B19" s="25">
+        <v>2.0570786199385549E-20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>1.8</v>
+      </c>
+      <c r="B20" s="25">
+        <v>9.1704348812836534E-20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
+        <v>1.9</v>
+      </c>
+      <c r="B21" s="25">
+        <v>3.9758398981011928E-19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>2</v>
+      </c>
+      <c r="B22" s="25">
+        <v>1.6742794102841391E-18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="B23" s="25">
+        <v>5.6319627453492627E-18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B24" s="25">
+        <v>2.2890844112484091E-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B25" s="25">
+        <v>8.9836295065324152E-17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="26">
+        <v>2.4</v>
+      </c>
+      <c r="B26" s="25">
+        <v>3.2980715135205582E-16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="B27" s="25">
+        <v>1.211369138988844E-15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="26">
+        <v>2.6</v>
+      </c>
+      <c r="B28" s="25">
+        <v>4.2926053041056307E-15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="26">
+        <v>2.7</v>
+      </c>
+      <c r="B29" s="25">
+        <v>1.4678968620234629E-14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="26">
+        <v>2.8</v>
+      </c>
+      <c r="B30" s="25">
+        <v>4.8455351664967378E-14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="26">
+        <v>2.9</v>
+      </c>
+      <c r="B31" s="25">
+        <v>1.5446666699861481E-13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="26">
+        <v>3</v>
+      </c>
+      <c r="B32" s="25">
+        <v>4.7574958665648038E-13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="26">
+        <v>3.1</v>
+      </c>
+      <c r="B33" s="25">
+        <v>1.4164476126868751E-12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="B34" s="25">
+        <v>4.119716010194322E-12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="26">
+        <v>3.3</v>
+      </c>
+      <c r="B35" s="25">
+        <v>1.146527124002392E-11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="26">
+        <v>3.4</v>
+      </c>
+      <c r="B36" s="25">
+        <v>3.0906897014683198E-11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="B37" s="25">
+        <v>8.0752591430672396E-11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="26">
+        <v>3.6</v>
+      </c>
+      <c r="B38" s="25">
+        <v>2.0463162906276579E-10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="26">
+        <v>3.7</v>
+      </c>
+      <c r="B39" s="25">
+        <v>5.0326465627917674E-10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="26">
+        <v>3.8</v>
+      </c>
+      <c r="B40" s="25">
+        <v>1.192104683073147E-9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="26">
+        <v>3.9</v>
+      </c>
+      <c r="B41" s="25">
+        <v>2.793607169863501E-9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="26">
+        <v>4</v>
+      </c>
+      <c r="B42" s="25">
+        <v>6.294907174398562E-9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="26">
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="B43" s="25">
+        <v>1.3832262112340489E-8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="26">
+        <v>4.2</v>
+      </c>
+      <c r="B44" s="25">
+        <v>2.9600231811612132E-8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="26">
+        <v>4.3</v>
+      </c>
+      <c r="B45" s="25">
+        <v>6.1729881435888253E-8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B46" s="25">
+        <v>1.252709746256171E-7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="26">
+        <v>4.5</v>
+      </c>
+      <c r="B47" s="25">
+        <v>2.4870253133855501E-7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="26">
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="B48" s="25">
+        <v>4.8213340896610669E-7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="26">
+        <v>4.7</v>
+      </c>
+      <c r="B49" s="25">
+        <v>9.1326965698466865E-7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="26">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="B50" s="25">
+        <v>1.6914438762268E-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B51" s="25">
+        <v>3.0693244955677289E-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="26">
+        <v>5</v>
+      </c>
+      <c r="B52" s="25">
+        <v>5.4434902345219387E-6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="26">
+        <v>5.1000000000000014</v>
+      </c>
+      <c r="B53" s="25">
+        <v>9.4572531690380029E-6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="26">
+        <v>5.2</v>
+      </c>
+      <c r="B54" s="25">
+        <v>1.6856012498792578E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="26">
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="B55" s="25">
+        <v>2.685411892021116E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="26">
+        <v>5.4</v>
+      </c>
+      <c r="B56" s="25">
+        <v>4.402368172482459E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="B57" s="25">
+        <v>7.0857167997530115E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="26">
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="B58" s="25">
+        <v>1.121014439304892E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="26">
+        <v>5.7</v>
+      </c>
+      <c r="B59" s="25">
+        <v>1.7418254688314149E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="26">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="B60" s="25">
+        <v>2.661424575654381E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="26">
+        <v>5.9</v>
+      </c>
+      <c r="B61" s="25">
+        <v>3.9978599657937571E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="26">
+        <v>6</v>
+      </c>
+      <c r="B62" s="25">
+        <v>5.9165580930264005E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="26">
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="B63" s="25">
+        <v>8.6227527796923196E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="26">
+        <v>6.2</v>
+      </c>
+      <c r="B64" s="25">
+        <v>1.2381071863207221E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="26">
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="B65" s="25">
+        <v>1.752976200446511E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="26">
+        <v>6.4</v>
+      </c>
+      <c r="B66" s="25">
+        <v>2.4463451838711409E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="26">
+        <v>6.5</v>
+      </c>
+      <c r="B67" s="25">
+        <v>3.367940568116185E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="26">
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="B68" s="25">
+        <v>4.5760973852781222E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="26">
+        <v>6.7</v>
+      </c>
+      <c r="B69" s="25">
+        <v>6.18744196393605E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="26">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="B70" s="25">
+        <v>8.1874249128331498E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="26">
+        <v>6.9</v>
+      </c>
+      <c r="B71" s="25">
+        <v>1.0706838469277939E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="26">
+        <v>7</v>
+      </c>
+      <c r="B72" s="25">
+        <v>1.384214000522407E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="26">
+        <v>7.1000000000000014</v>
+      </c>
+      <c r="B73" s="25">
+        <v>1.7697846002829112E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="26">
+        <v>7.2</v>
+      </c>
+      <c r="B74" s="25">
+        <v>2.2384983580172879E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="26">
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="B75" s="25">
+        <v>2.8019045457301529E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="26">
+        <v>7.4</v>
+      </c>
+      <c r="B76" s="25">
+        <v>3.4717477059230818E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="26">
+        <v>7.5</v>
+      </c>
+      <c r="B77" s="25">
+        <v>4.2596753947629747E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="26">
+        <v>7.6000000000000014</v>
+      </c>
+      <c r="B78" s="25">
+        <v>5.1769136230229412E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="26">
+        <v>7.7</v>
+      </c>
+      <c r="B79" s="25">
+        <v>6.2339211901870348E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="26">
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="B80" s="25">
+        <v>7.44003610944413E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="26">
+        <v>7.9</v>
+      </c>
+      <c r="B81" s="25">
+        <v>8.8031286424665081E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="26">
+        <v>8</v>
+      </c>
+      <c r="B82" s="25">
+        <v>0.1032927597948442</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="26">
+        <v>8.1</v>
+      </c>
+      <c r="B83" s="25">
+        <v>0.1202247324292291</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="26">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="B84" s="25">
+        <v>0.13884394296536209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="26">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B85" s="25">
+        <v>0.1591421383909723</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="26">
+        <v>8.4</v>
+      </c>
+      <c r="B86" s="25">
+        <v>0.1810849961322458</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="B87" s="25">
+        <v>0.204611804144776</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="26">
+        <v>8.6</v>
+      </c>
+      <c r="B88" s="25">
+        <v>0.22963592156724399</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="26">
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="B89" s="25">
+        <v>0.25604600746771677</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="26">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B90" s="25">
+        <v>0.28370797157421568</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="26">
+        <v>8.9</v>
+      </c>
+      <c r="B91" s="25">
+        <v>0.31246757058787528</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="26">
+        <v>9</v>
+      </c>
+      <c r="B92" s="25">
+        <v>0.34453104178391619</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="26">
+        <v>9.1</v>
+      </c>
+      <c r="B93" s="25">
+        <v>0.37401465984871612</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="26">
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="B94" s="25">
+        <v>0.40425461155954862</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="26">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B95" s="25">
+        <v>0.43507797112239049</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="26">
+        <v>9.4</v>
+      </c>
+      <c r="B96" s="25">
+        <v>0.46630117135281529</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="26">
+        <v>9.5</v>
+      </c>
+      <c r="B97" s="25">
+        <v>0.49773327285958968</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="26">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="B98" s="25">
+        <v>0.52917945930312738</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="26">
+        <v>9.7000000000000011</v>
+      </c>
+      <c r="B99" s="25">
+        <v>0.56044465232528673</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="26">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B100" s="25">
+        <v>0.59133713458615977</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="26">
+        <v>9.9</v>
+      </c>
+      <c r="B101" s="25">
+        <v>0.62167206899302896</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="26">
+        <v>10</v>
+      </c>
+      <c r="B102" s="25">
+        <v>0.64766120625967805</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="26">
+        <v>10.1</v>
+      </c>
+      <c r="B103" s="25">
+        <v>0.6751166489991125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="26">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B104" s="25">
+        <v>0.70144611626973452</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="26">
+        <v>10.3</v>
+      </c>
+      <c r="B105" s="25">
+        <v>0.72656507281253113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="26">
+        <v>10.4</v>
+      </c>
+      <c r="B106" s="25">
+        <v>0.75040810962597726</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="26">
+        <v>10.5</v>
+      </c>
+      <c r="B107" s="25">
+        <v>0.77292844852617315</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="26">
+        <v>10.6</v>
+      </c>
+      <c r="B108" s="25">
+        <v>0.79409709026140896</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="26">
+        <v>10.7</v>
+      </c>
+      <c r="B109" s="25">
+        <v>0.813901667605331</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="26">
+        <v>10.8</v>
+      </c>
+      <c r="B110" s="25">
+        <v>0.83234506685769327</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="26">
+        <v>10.9</v>
+      </c>
+      <c r="B111" s="25">
+        <v>0.84944388056526221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="26">
+        <v>11</v>
+      </c>
+      <c r="B112" s="25">
+        <v>0.86522675149758033</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="26">
+        <v>11.1</v>
+      </c>
+      <c r="B113" s="25">
+        <v>0.87973266325760457</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="26">
+        <v>11.2</v>
+      </c>
+      <c r="B114" s="25">
+        <v>0.89300922711676334</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="26">
+        <v>11.3</v>
+      </c>
+      <c r="B115" s="25">
+        <v>0.90511100781264398</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="26">
+        <v>11.4</v>
+      </c>
+      <c r="B116" s="25">
+        <v>0.91609792389621525</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="26">
+        <v>11.5</v>
+      </c>
+      <c r="B117" s="25">
+        <v>0.92603375087726869</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="26">
+        <v>11.6</v>
+      </c>
+      <c r="B118" s="25">
+        <v>0.93498474828486522</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="26">
+        <v>11.7</v>
+      </c>
+      <c r="B119" s="25">
+        <v>0.94301842507776268</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="26">
+        <v>11.8</v>
+      </c>
+      <c r="B120" s="25">
+        <v>0.95020245177840723</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="26">
+        <v>11.9</v>
+      </c>
+      <c r="B121" s="25">
+        <v>0.95660372234462343</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="26">
+        <v>12</v>
+      </c>
+      <c r="B122" s="25">
+        <v>0.96228756423360029</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="26">
+        <v>12.1</v>
+      </c>
+      <c r="B123" s="25">
+        <v>0.96731709142317801</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="26">
+        <v>12.2</v>
+      </c>
+      <c r="B124" s="25">
+        <v>0.97175269224232597</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="26">
+        <v>12.3</v>
+      </c>
+      <c r="B125" s="25">
+        <v>0.9756516416178761</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="26">
+        <v>12.4</v>
+      </c>
+      <c r="B126" s="25">
+        <v>0.97892285868074491</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="26">
+        <v>12.5</v>
+      </c>
+      <c r="B127" s="25">
+        <v>0.98190832883536205</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="26">
+        <v>12.6</v>
+      </c>
+      <c r="B128" s="25">
+        <v>0.98450896775490304</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="26">
+        <v>12.7</v>
+      </c>
+      <c r="B129" s="25">
+        <v>0.9867676910043075</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="26">
+        <v>12.8</v>
+      </c>
+      <c r="B130" s="25">
+        <v>0.98872378749870671</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="26">
+        <v>12.9</v>
+      </c>
+      <c r="B131" s="25">
+        <v>0.99041302124218089</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="26">
+        <v>13</v>
+      </c>
+      <c r="B132" s="25">
+        <v>0.99186777229663448</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="26">
+        <v>13.1</v>
+      </c>
+      <c r="B133" s="25">
+        <v>0.99311720721080532</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="26">
+        <v>13.2</v>
+      </c>
+      <c r="B134" s="25">
+        <v>0.99418747025747822</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="26">
+        <v>13.3</v>
+      </c>
+      <c r="B135" s="25">
+        <v>0.9951018879837723</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="26">
+        <v>13.4</v>
+      </c>
+      <c r="B136" s="25">
+        <v>0.99588118069786025</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="26">
+        <v>13.5</v>
+      </c>
+      <c r="B137" s="25">
+        <v>0.99654367558582868</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="26">
+        <v>13.6</v>
+      </c>
+      <c r="B138" s="25">
+        <v>0.99710551715025875</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="26">
+        <v>13.7</v>
+      </c>
+      <c r="B139" s="25">
+        <v>0.99758087156621145</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="26">
+        <v>13.8</v>
+      </c>
+      <c r="B140" s="25">
+        <v>0.99798212236013795</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="26">
+        <v>13.9</v>
+      </c>
+      <c r="B141" s="25">
+        <v>0.99832005552597991</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="26">
+        <v>14</v>
+      </c>
+      <c r="B142" s="25">
+        <v>0.99860403280151044</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="26">
+        <v>14.1</v>
+      </c>
+      <c r="B143" s="25">
+        <v>0.99884215234152873</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="26">
+        <v>14.2</v>
+      </c>
+      <c r="B144" s="25">
+        <v>0.99904139644804335</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="26">
+        <v>14.3</v>
+      </c>
+      <c r="B145" s="25">
+        <v>0.99920776636061648</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="26">
+        <v>14.4</v>
+      </c>
+      <c r="B146" s="25">
+        <v>0.99934640437773481</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="26">
+        <v>14.5</v>
+      </c>
+      <c r="B147" s="25">
+        <v>0.99946170378504429</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="26">
+        <v>14.6</v>
+      </c>
+      <c r="B148" s="25">
+        <v>0.99955740721508191</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="26">
+        <v>14.7</v>
+      </c>
+      <c r="B149" s="25">
+        <v>0.99963669416368139</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="26">
+        <v>14.8</v>
+      </c>
+      <c r="B150" s="25">
+        <v>0.99970225845094696</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="26">
+        <v>14.9</v>
+      </c>
+      <c r="B151" s="25">
+        <v>0.99975637644491222</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="26">
+        <v>15</v>
+      </c>
+      <c r="B152" s="25">
+        <v>0.99980096687025477</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="26">
+        <v>15.1</v>
+      </c>
+      <c r="B153" s="25">
+        <v>0.99983764300966371</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="26">
+        <v>15.2</v>
+      </c>
+      <c r="B154" s="25">
+        <v>0.99986741029323545</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="26">
+        <v>15.3</v>
+      </c>
+      <c r="B155" s="25">
+        <v>0.99989214544951066</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="26">
+        <v>15.4</v>
+      </c>
+      <c r="B156" s="25">
+        <v>0.99991239131016629</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="26">
+        <v>15.5</v>
+      </c>
+      <c r="B157" s="25">
+        <v>0.99992893622370416</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="26">
+        <v>15.6</v>
+      </c>
+      <c r="B158" s="25">
+        <v>0.99994243561474949</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="26">
+        <v>15.7</v>
+      </c>
+      <c r="B159" s="25">
+        <v>0.99995343325955655</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="26">
+        <v>15.8</v>
+      </c>
+      <c r="B160" s="25">
+        <v>0.99996237938811039</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="26">
+        <v>15.9</v>
+      </c>
+      <c r="B161" s="25">
+        <v>0.99996964603913574</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="26">
+        <v>16</v>
+      </c>
+      <c r="B162" s="25">
+        <v>0.99997554004664924</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="26">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B163" s="25">
+        <v>0.9999803139923098</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="26">
+        <v>16.2</v>
+      </c>
+      <c r="B164" s="25">
+        <v>0.99998417541700246</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="26">
+        <v>16.3</v>
+      </c>
+      <c r="B165" s="25">
+        <v>0.99998729454794477</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="26">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="B166" s="25">
+        <v>0.99998981076405746</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="26">
+        <v>16.5</v>
+      </c>
+      <c r="B167" s="25">
+        <v>0.99999183799233349</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="26">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="B168" s="25">
+        <v>0.99999346920124965</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="26">
+        <v>16.7</v>
+      </c>
+      <c r="B169" s="25">
+        <v>0.99999478013369236</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="26">
+        <v>16.8</v>
+      </c>
+      <c r="B170" s="25">
+        <v>0.99999583240120482</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="26">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B171" s="25">
+        <v>0.99999667604328046</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="26">
+        <v>17</v>
+      </c>
+      <c r="B172" s="25">
+        <v>0.99999735163975922</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="26">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B173" s="25">
+        <v>0.99999789205082124</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="26">
+        <v>17.2</v>
+      </c>
+      <c r="B174" s="25">
+        <v>0.99999832384739995</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="26">
+        <v>17.3</v>
+      </c>
+      <c r="B175" s="25">
+        <v>0.99999867118028818</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="26">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="B176" s="25">
+        <v>0.9999989454905055</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="26">
+        <v>17.5</v>
+      </c>
+      <c r="B177" s="25">
+        <v>0.9999991639536433</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="26">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="B178" s="25">
+        <v>0.99999933776219263</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="26">
+        <v>17.7</v>
+      </c>
+      <c r="B179" s="25">
+        <v>0.99999947590563099</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="26">
+        <v>17.8</v>
+      </c>
+      <c r="B180" s="25">
+        <v>0.99999958559504842</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="26">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="B181" s="25">
+        <v>0.99999967260792699</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="26">
+        <v>18</v>
+      </c>
+      <c r="B182" s="25">
+        <v>0.9999997415676477</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="26">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B183" s="25">
+        <v>0.99999979616973411</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="26">
+        <v>18.2</v>
+      </c>
+      <c r="B184" s="25">
+        <v>0.99999983936470949</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="26">
+        <v>18.3</v>
+      </c>
+      <c r="B185" s="25">
+        <v>0.99999987350567188</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="26">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="B186" s="25">
+        <v>0.99999990046722798</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="26">
+        <v>18.5</v>
+      </c>
+      <c r="B187" s="25">
+        <v>0.99999992174120944</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="26">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="B188" s="25">
+        <v>0.99999993851360225</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="26">
+        <v>18.7</v>
+      </c>
+      <c r="B189" s="25">
+        <v>0.99999995172629574</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="26">
+        <v>18.8</v>
+      </c>
+      <c r="B190" s="25">
+        <v>0.99999996212658149</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="26">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="B191" s="25">
+        <v>0.99999997030678511</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="26">
+        <v>19</v>
+      </c>
+      <c r="B192" s="25">
+        <v>0.99999997673595797</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="26">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B193" s="25">
+        <v>0.99999998178518956</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="26">
+        <v>19.2</v>
+      </c>
+      <c r="B194" s="25">
+        <v>0.99999998574780213</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="26">
+        <v>19.3</v>
+      </c>
+      <c r="B195" s="25">
+        <v>0.99999998885544328</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="26">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="B196" s="25">
+        <v>0.99999999129089601</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="26">
+        <v>19.5</v>
+      </c>
+      <c r="B197" s="25">
+        <v>0.99999999319826482</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="26">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="B198" s="25">
+        <v>0.99999999469106671</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="26">
+        <v>19.7</v>
+      </c>
+      <c r="B199" s="25">
+        <v>0.99999999585865162</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="26">
+        <v>19.8</v>
+      </c>
+      <c r="B200" s="25">
+        <v>0.99999999677129225</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="26">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="B201" s="25">
+        <v>0.99999999748421442</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="26">
+        <v>20</v>
+      </c>
+      <c r="B202" s="25">
+        <v>0.99999999804078654</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521A9E3A-32A5-4F7F-BDC5-66483993CE3B}">
   <dimension ref="A1:F202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>